<commit_message>
Added monthly download & daily row entry
</commit_message>
<xml_diff>
--- a/excel/S&T BT February bill 2026.xlsx
+++ b/excel/S&T BT February bill 2026.xlsx
@@ -728,15 +728,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1064,17 +1064,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
+      <c r="A1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
@@ -1153,7 +1153,7 @@
       <c r="H6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="58" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1178,7 +1178,7 @@
       <c r="H7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="62"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="32">
@@ -1778,8 +1778,8 @@
     <mergeCell ref="A45:D45"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="E4:I4"/>
@@ -1826,17 +1826,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
+      <c r="A1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
@@ -1915,7 +1915,7 @@
       <c r="H6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="58" t="s">
         <v>13</v>
       </c>
       <c r="L6" s="22"/>
@@ -1941,7 +1941,7 @@
       <c r="H7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="62"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="32">
@@ -2563,8 +2563,8 @@
     <mergeCell ref="A45:D45"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="E4:I4"/>
@@ -2611,17 +2611,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="60"/>
+      <c r="A1" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="62"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="48" t="s">
@@ -2700,7 +2700,7 @@
       <c r="H6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="58" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2725,7 +2725,7 @@
       <c r="H7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="62"/>
+      <c r="I7" s="59"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="32">
@@ -3325,8 +3325,8 @@
     <mergeCell ref="A45:D45"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="F5:I5"/>
+    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="I6:I7"/>
     <mergeCell ref="A42:D42"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="E4:I4"/>

</xml_diff>